<commit_message>
Updated Cost Estimate Sheet
</commit_message>
<xml_diff>
--- a/USB433-BOM-Cost-Estimate.xlsx
+++ b/USB433-BOM-Cost-Estimate.xlsx
@@ -1,46 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DS1821plus\documents\03-Hobbies &amp; Projects\15-Business Products\433MHz-SRX882S-Dongle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DS1821plus\documents\03-Hobbies &amp; Projects\15-Business Products\0002-STM32-433MHz-SxX882S\_GIT Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D332C820-9C1C-4025-B84C-8D0FC855E221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3120CB-6472-441D-956A-FA4B3E55A342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9780066-9491-4589-8172-5297DED98AE2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D9780066-9491-4589-8172-5297DED98AE2}"/>
   </bookViews>
   <sheets>
     <sheet name="433MHz-SRX882S-Dongle" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="148">
-  <si>
-    <t>Source:</t>
-  </si>
-  <si>
-    <t>\\DS1821plus\documents\03-Hobbies &amp; Projects\15-Business Products\433MHz-SRX882S-Dongle\433MHz-SRX882S-Dongle.kicad_sch</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="143">
   <si>
     <t>Tool:</t>
   </si>
   <si>
     <t>Eeschema (6.0.11)</t>
-  </si>
-  <si>
-    <t>Generator:</t>
-  </si>
-  <si>
-    <t>C:\Program Files\KiCad\6.0\bin\scripting\plugins/bom_csv_grouped_by_value_with_fp.py</t>
   </si>
   <si>
     <t>Component Count:</t>
@@ -472,7 +468,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -958,14 +954,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1322,22 +1317,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79C9DC9-A2D1-4834-9AEF-1ACAE5A66884}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="93.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1354,8 +1349,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>45806.363622685189</v>
+      <c r="B2">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1365,182 +1360,257 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.04E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <f>G4*B4</f>
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.1802</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H26" si="0">G5*B5</f>
+        <v>0.1802</v>
+      </c>
+      <c r="I5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>112</v>
+        <v>14</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>8.4999999999999989E-3</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="J6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1.04E-2</v>
-      </c>
-      <c r="H7" s="3">
-        <f>G7*B7</f>
-        <v>2.0799999999999999E-2</v>
+        <v>14</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="I7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.1802</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" ref="H8:H32" si="0">G8*B8</f>
-        <v>0.1802</v>
+        <v>14</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="I8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
-        <v>8.4999999999999989E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="I9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3">
-        <v>2.4799999999999999E-2</v>
-      </c>
-      <c r="H10" s="3">
+        <v>33</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>2.4799999999999999E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="I10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J10" t="s">
         <v>116</v>
@@ -1548,32 +1618,32 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>33</v>
       </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3">
-        <v>5.1999999999999998E-3</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G11" s="2">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>5.1999999999999998E-3</v>
+        <v>2.3900000000000001E-2</v>
       </c>
       <c r="I11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J11" t="s">
         <v>117</v>
@@ -1581,32 +1651,32 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="H12" s="3">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>2.3999999999999998E-3</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J12" t="s">
         <v>118</v>
@@ -1614,458 +1684,454 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="2">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" t="s">
         <v>119</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="3">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7100000000000001E-2</v>
-      </c>
-      <c r="I13" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="3">
-        <v>2.3900000000000001E-2</v>
-      </c>
-      <c r="H14" s="3">
+        <v>48</v>
+      </c>
+      <c r="H14" s="2">
         <f t="shared" si="0"/>
-        <v>2.3900000000000001E-2</v>
-      </c>
-      <c r="I14" t="s">
-        <v>110</v>
-      </c>
-      <c r="J14" t="s">
-        <v>122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="3">
-        <v>4.1000000000000003E-3</v>
-      </c>
-      <c r="H15" s="3">
+        <v>51</v>
+      </c>
+      <c r="G15" s="5">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="H15" s="2">
         <f t="shared" si="0"/>
-        <v>4.1000000000000003E-3</v>
+        <v>6.6199999999999995E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="3">
-        <v>7.6100000000000001E-2</v>
-      </c>
-      <c r="H16" s="3">
+        <v>55</v>
+      </c>
+      <c r="H16" s="2">
         <f t="shared" si="0"/>
-        <v>7.6100000000000001E-2</v>
-      </c>
-      <c r="I16" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" t="s">
-        <v>124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="3">
+        <v>60</v>
+      </c>
+      <c r="H17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="6">
-        <v>3.3099999999999997E-2</v>
-      </c>
-      <c r="H18" s="3">
+        <v>60</v>
+      </c>
+      <c r="H18" s="2">
         <f t="shared" si="0"/>
-        <v>6.6199999999999995E-2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>110</v>
-      </c>
-      <c r="J18" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="3">
+        <v>67</v>
+      </c>
+      <c r="G19" s="5">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="H19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="3">
+        <v>71</v>
+      </c>
+      <c r="G20" s="2">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="H20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="3">
+        <v>71</v>
+      </c>
+      <c r="G21" s="2">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="H21" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
       </c>
       <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
         <v>71</v>
       </c>
-      <c r="F22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="6">
-        <v>2.3300000000000001E-2</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="G22" s="2">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="H22" s="2">
         <f t="shared" si="0"/>
-        <v>2.3300000000000001E-2</v>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="I22" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="3">
-        <v>7.7000000000000002E-3</v>
-      </c>
-      <c r="H23" s="3">
+        <v>71</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="H23" s="2">
         <f t="shared" si="0"/>
-        <v>7.7000000000000002E-3</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="I23" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="3">
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="H24" s="3">
+        <v>82</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="H24" s="2">
         <f t="shared" si="0"/>
-        <v>3.9199999999999999E-2</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="I24" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="3">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="H25" s="3">
+        <v>85</v>
+      </c>
+      <c r="G25" s="2">
+        <f>14.99/8</f>
+        <v>1.87375</v>
+      </c>
+      <c r="H25" s="2">
         <f t="shared" si="0"/>
-        <v>1.5599999999999999E-2</v>
+        <v>1.87375</v>
       </c>
       <c r="I25" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="J25" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="H26" s="3">
+        <v>90</v>
+      </c>
+      <c r="G26" s="2">
+        <v>7.22E-2</v>
+      </c>
+      <c r="H26" s="2">
         <f t="shared" si="0"/>
-        <v>5.1000000000000004E-2</v>
+        <v>7.22E-2</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="3">
-        <v>1.2200000000000001E-2</v>
-      </c>
-      <c r="H27" s="3">
-        <f t="shared" si="0"/>
-        <v>1.2200000000000001E-2</v>
+        <v>93</v>
+      </c>
+      <c r="G27" s="2">
+        <f>14.99/8</f>
+        <v>1.87375</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" ref="H27" si="1">G27*B27</f>
+        <v>1.87375</v>
       </c>
       <c r="I27" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="J27" t="s">
         <v>135</v>
@@ -2073,263 +2139,168 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>90</v>
-      </c>
-      <c r="G28" s="3">
-        <f>14.99/8</f>
-        <v>1.87375</v>
-      </c>
-      <c r="H28" s="3">
-        <f t="shared" si="0"/>
-        <v>1.87375</v>
+        <v>96</v>
+      </c>
+      <c r="F28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1.7009000000000001</v>
+      </c>
+      <c r="H28" s="2">
+        <f>G28*B27</f>
+        <v>1.7009000000000001</v>
       </c>
       <c r="I28" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="J28" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G29" s="3">
-        <v>7.22E-2</v>
-      </c>
-      <c r="H29" s="3">
-        <f t="shared" si="0"/>
-        <v>7.22E-2</v>
+        <v>102</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.2056</v>
+      </c>
+      <c r="H29" s="2">
+        <f>G29*B28</f>
+        <v>0.2056</v>
       </c>
       <c r="I29" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="3">
-        <f>14.99/8</f>
-        <v>1.87375</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" ref="H30" si="1">G30*B30</f>
-        <v>1.87375</v>
-      </c>
-      <c r="I30" t="s">
-        <v>139</v>
-      </c>
-      <c r="J30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1.7009000000000001</v>
-      </c>
-      <c r="H31" s="3">
-        <f>G31*B30</f>
-        <v>1.7009000000000001</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="H31" s="2">
+        <f>SUM(H4:H29)</f>
+        <v>6.3044999999999991</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G32" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J31" t="s">
+      <c r="H32" s="2">
+        <f>SUM(M35:M43) / SUM(N35:N43)</f>
+        <v>4.7666666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G33" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>103</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0.2056</v>
-      </c>
-      <c r="H32" s="3">
-        <f>G32*B31</f>
-        <v>0.2056</v>
-      </c>
-      <c r="I32" t="s">
-        <v>110</v>
-      </c>
-      <c r="J32" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G34" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H34" s="3">
-        <f>SUM(H7:H32)</f>
-        <v>6.3044999999999991</v>
-      </c>
-    </row>
-    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G35" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H35" s="3">
-        <f>SUM(M38:M46) / SUM(N38:N46)</f>
-        <v>4.7666666666666666</v>
-      </c>
-    </row>
-    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G36" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="H36" s="3">
-        <f>I36/SUM(N38:N46)</f>
+      <c r="H33" s="2">
+        <f>I33/SUM(N35:N43)</f>
         <v>9.69</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I33" s="1">
         <f>24.01+5.06</f>
         <v>29.07</v>
       </c>
     </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H34" s="2">
+        <f>SUM(H31:H33)</f>
+        <v>20.761166666666668</v>
+      </c>
+      <c r="K34" t="s">
+        <v>142</v>
+      </c>
+      <c r="L34" t="s">
+        <v>141</v>
+      </c>
+      <c r="M34" t="s">
+        <v>139</v>
+      </c>
+      <c r="N34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35" s="1">
+        <v>14.3</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36" s="3"/>
+    </row>
     <row r="37" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="H37" s="3">
-        <f>SUM(H34:H36)</f>
-        <v>20.761166666666668</v>
-      </c>
-      <c r="K37" t="s">
-        <v>147</v>
-      </c>
-      <c r="L37" t="s">
-        <v>146</v>
-      </c>
-      <c r="M37" t="s">
-        <v>144</v>
-      </c>
-      <c r="N37" t="s">
-        <v>145</v>
+      <c r="L37">
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="7:14" x14ac:dyDescent="0.25">
       <c r="L38">
-        <v>1</v>
-      </c>
-      <c r="M38" s="2">
-        <v>14.3</v>
-      </c>
-      <c r="N38">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="7:14" x14ac:dyDescent="0.25">
       <c r="L39">
-        <v>2</v>
-      </c>
-      <c r="M39" s="4"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="7:14" x14ac:dyDescent="0.25">
       <c r="L40">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="7:14" x14ac:dyDescent="0.25">
       <c r="L41">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="7:14" x14ac:dyDescent="0.25">
       <c r="L42">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="7:14" x14ac:dyDescent="0.25">
       <c r="L43">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="L44">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="L45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="L46">
         <v>9</v>
       </c>
     </row>

</xml_diff>